<commit_message>
Toevoegen van voorbeeld 2 en 3
</commit_message>
<xml_diff>
--- a/Leden van activiteit.xlsx
+++ b/Leden van activiteit.xlsx
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\@@ Python\Projectjes\Git\Mailclient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02B4FE6-12DA-44D4-9036-2CA14A51C16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D169C1E0-DA4A-4CBF-8989-A2838192109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -426,7 +438,7 @@
   <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Toevoegen code voor check dubbele
</commit_message>
<xml_diff>
--- a/Leden van activiteit.xlsx
+++ b/Leden van activiteit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\@@ Python\Projectjes\Git\Mailclient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D169C1E0-DA4A-4CBF-8989-A2838192109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD66F8E-814C-4F5D-8531-72F7A994B109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6600" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,13 +110,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,7 +440,7 @@
   <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C5"/>
+      <selection activeCell="A5" sqref="A5:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,16 +455,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -515,13 +517,30 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>

</xml_diff>